<commit_message>
Acceptatie Test en Moscow gemaakt
</commit_message>
<xml_diff>
--- a/doc/Aanvullende taken/MyVending - WBS.xlsx
+++ b/doc/Aanvullende taken/MyVending - WBS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxvd\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxvd\Desktop\Proftaak2018\doc\Aanvullende taken\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E61E436C-3ABC-4521-9936-E91DD94CDEE9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8125E233-7D3B-4F24-9F55-C8EF1C11D8AE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,21 +18,26 @@
     <sheet name="version" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'#PROJECTNAME#'!$A$4:$J$18</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'#PROJECTNAME#'!$A$1:$J$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'#PROJECTNAME#'!$A$4:$J$81</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'#PROJECTNAME#'!$A$1:$J$82</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="139">
   <si>
     <t>totaal</t>
   </si>
@@ -403,6 +408,57 @@
   </si>
   <si>
     <t>Windows crash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remote access </t>
+  </si>
+  <si>
+    <t>Interview</t>
+  </si>
+  <si>
+    <t>Mjak</t>
+  </si>
+  <si>
+    <t>Project plan</t>
+  </si>
+  <si>
+    <t>Kerntaken</t>
+  </si>
+  <si>
+    <t>Mboo/Mjak</t>
+  </si>
+  <si>
+    <t>Technisch ontwerp</t>
+  </si>
+  <si>
+    <t>Functioneel ontwerp</t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>Examen portfolio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WBS </t>
+  </si>
+  <si>
+    <t>Fancy poster</t>
+  </si>
+  <si>
+    <t>Technisch poster</t>
+  </si>
+  <si>
+    <t>CRPR lijst</t>
+  </si>
+  <si>
+    <t>Test lijst</t>
+  </si>
+  <si>
+    <t>Acceptatie test</t>
+  </si>
+  <si>
+    <t>Evaluatie verslag</t>
   </si>
 </sst>
 </file>
@@ -656,7 +712,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -934,10 +990,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I71" sqref="I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -946,7 +1002,7 @@
     <col min="2" max="2" width="11.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="43.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40.85546875" style="19" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="10.7109375" style="1" customWidth="1" outlineLevel="1"/>
     <col min="9" max="10" width="34.5703125" style="1" customWidth="1" outlineLevel="1"/>
@@ -1103,10 +1159,10 @@
         <v>80</v>
       </c>
       <c r="G8" s="1">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="H8" s="1">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1877,10 +1933,10 @@
         <v>102</v>
       </c>
       <c r="G46" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H46" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -1960,10 +2016,10 @@
         <v>97</v>
       </c>
       <c r="G50" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H50" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -2068,7 +2124,7 @@
         <v>6</v>
       </c>
       <c r="H56" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -2119,10 +2175,10 @@
         <v>97</v>
       </c>
       <c r="G59" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H59" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -2208,118 +2264,355 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="24">
-        <f ca="1">+A64:IA64:J64</f>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>39</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="G64" s="1">
+        <v>2</v>
+      </c>
+      <c r="H64" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="24">
+        <f ca="1">+A65:IA65:J65</f>
         <v>0</v>
       </c>
-      <c r="B64" s="24"/>
-      <c r="C64" s="27" t="s">
+      <c r="B65" s="24"/>
+      <c r="C65" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="D64" s="25"/>
-      <c r="E64" s="26"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="25"/>
-      <c r="H64" s="25"/>
-      <c r="I64" s="25"/>
-      <c r="J64" s="25"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
-        <v>40</v>
-      </c>
+      <c r="D65" s="25"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="25"/>
+      <c r="G65" s="25"/>
+      <c r="H65" s="25"/>
+      <c r="I65" s="25"/>
+      <c r="J65" s="25"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E66" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="G66" s="1">
+        <v>2</v>
+      </c>
+      <c r="H66" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E67" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="G67" s="1">
+        <v>5</v>
+      </c>
+      <c r="H67" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>43</v>
-      </c>
-      <c r="I68" s="1">
-        <f>SUM(H7:H35)</f>
-        <v>66.8</v>
+        <v>42</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="G68" s="1">
+        <v>6</v>
+      </c>
+      <c r="H68" s="1">
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>44</v>
-      </c>
-      <c r="I69" s="1">
-        <f>SUM(H44:H61)</f>
-        <v>96</v>
+        <v>43</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E69" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="G69" s="1">
+        <v>8</v>
+      </c>
+      <c r="H69" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E70" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="G70" s="1">
+        <v>8</v>
+      </c>
+      <c r="H70" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E71" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="G71" s="1">
+        <v>4</v>
+      </c>
+      <c r="H71" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E72" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="G72" s="1">
+        <v>8</v>
+      </c>
+      <c r="H72" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E73" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="G73" s="1">
+        <v>2</v>
+      </c>
+      <c r="H73" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E74" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="G74" s="1">
+        <v>4</v>
+      </c>
+      <c r="H74" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E75" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="G75" s="1">
+        <v>4</v>
+      </c>
+      <c r="H75" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E76" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="G76" s="1">
+        <v>2</v>
+      </c>
+      <c r="H76" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
+        <v>51</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E77" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="G77" s="1">
+        <v>2</v>
+      </c>
+      <c r="H77" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
         <v>52</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="2"/>
-      <c r="B78" s="2"/>
-      <c r="C78" s="2" t="s">
+      <c r="C78" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E78" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="G78" s="1">
+        <v>2</v>
+      </c>
+      <c r="H78" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>53</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E79" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="G79" s="1">
+        <v>4</v>
+      </c>
+      <c r="H79" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="2"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D78" s="2"/>
-      <c r="E78" s="14"/>
-      <c r="F78" s="20"/>
-      <c r="G78" s="20">
-        <f>SUBTOTAL(9,G7:G77)</f>
-        <v>178.8</v>
-      </c>
-      <c r="H78" s="2">
-        <f>SUM(H7:H41)</f>
-        <v>90.8</v>
-      </c>
-      <c r="I78" s="2"/>
-      <c r="J78" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="20"/>
+      <c r="G82" s="20">
+        <f>SUBTOTAL(9,G7:G79)</f>
+        <v>230</v>
+      </c>
+      <c r="H82" s="2">
+        <f>SUM(H7:H79)</f>
+        <v>240</v>
+      </c>
+      <c r="I82" s="2"/>
+      <c r="J82" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:J18" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A4:J81" xr:uid="{295828EB-444F-4471-B776-D113FBAB1DE5}"/>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>

</xml_diff>